<commit_message>
Improved Notifications and minnor bug fixes
</commit_message>
<xml_diff>
--- a/reports_data/generated_report.xlsx
+++ b/reports_data/generated_report.xlsx
@@ -592,7 +592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,6 +719,146 @@
       <c r="D6" t="inlineStr">
         <is>
           <t>Matematica</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>suficiencia</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>premio</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>suficiencia</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>suficiencia</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>suficiencia</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nom</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>premio</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>sd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>suficiencia</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>grt</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1198,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-09 13:35:13</t>
+          <t>2025-06-09 14:16:57</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1249,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -1119,7 +1259,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -1129,7 +1269,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">

</xml_diff>